<commit_message>
Updated Eagle Lake Ice-Out post
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/IceDates.xlsx
+++ b/portfolio/posts/_data/IceDates.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaaPersonal\Vis_Fun\Lake_Ice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaaWork\Web\droglenc.github.io\portfolio\posts\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="11" activeTab="22"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="7" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Nebagamon" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="283">
   <si>
     <t>iceOut</t>
   </si>
@@ -1074,9 +1074,6 @@
     <t>Crystal Lake WI … from a query at https://nsidc.org/data/lake_river_ice/freezethaw.html</t>
   </si>
   <si>
-    <t>Lake Mendota WI … from a query at https://nsidc.org/data/lake_river_ice/freezethaw.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Note that this includes data for when the ice came in, went out, and came back</t>
   </si>
   <si>
@@ -1108,6 +1105,15 @@
   </si>
   <si>
     <t>Maple Lake WI … from a query at https://nsidc.org/data/lake_river_ice/freezethaw.html</t>
+  </si>
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>2022-23</t>
+  </si>
+  <si>
+    <t>Lake Mendota WI … from a query at https://nsidc.org/data/lake_river_ice/freezethaw.html and from https://www.aos.wisc.edu/~sco/lakes/Mendota-ice.html</t>
   </si>
 </sst>
 </file>
@@ -1534,8 +1540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+    <sheetView topLeftCell="A61" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A61" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5978,7 +5984,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -7928,9 +7934,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C170"/>
+  <dimension ref="A1:C174"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -7940,12 +7948,12 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -9777,6 +9785,50 @@
       </c>
       <c r="C170" s="1">
         <v>44651</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" t="s">
+        <v>251</v>
+      </c>
+      <c r="B171" s="1">
+        <v>44938</v>
+      </c>
+      <c r="C171" s="1">
+        <v>45007</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" t="s">
+        <v>252</v>
+      </c>
+      <c r="B172" s="1">
+        <v>44929</v>
+      </c>
+      <c r="C172" s="1">
+        <v>45005</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" t="s">
+        <v>253</v>
+      </c>
+      <c r="B173" s="1">
+        <v>44933</v>
+      </c>
+      <c r="C173" s="1">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" t="s">
+        <v>281</v>
+      </c>
+      <c r="B174" s="1">
+        <v>45285</v>
+      </c>
+      <c r="C174" s="1">
+        <v>45018</v>
       </c>
     </row>
   </sheetData>
@@ -9800,7 +9852,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -9816,7 +9868,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B5" s="1">
         <v>44908</v>
@@ -11659,7 +11711,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -12067,7 +12119,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -12886,7 +12938,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -13551,10 +13603,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13757,6 +13809,14 @@
       </c>
       <c r="C27" s="1">
         <v>44687</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>280</v>
+      </c>
+      <c r="C28" s="1">
+        <v>45050</v>
       </c>
     </row>
   </sheetData>
@@ -13779,7 +13839,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -14124,7 +14184,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -14626,7 +14686,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -15129,7 +15189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -15139,7 +15199,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:3">

</xml_diff>

<commit_message>
Mostly added to the dam heights post
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/IceDates.xlsx
+++ b/portfolio/posts/_data/IceDates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="2" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Nebagamon" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="285">
   <si>
     <t>iceOut</t>
   </si>
@@ -1544,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A61" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2427,6 +2427,39 @@
       </c>
       <c r="C82" s="1">
         <v>44655</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" s="1">
+        <v>45632</v>
+      </c>
+      <c r="C83" s="1">
+        <v>45417</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>280</v>
+      </c>
+      <c r="B84" s="1">
+        <v>45633</v>
+      </c>
+      <c r="C84" s="1">
+        <v>45416</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>282</v>
+      </c>
+      <c r="B85" s="1">
+        <v>45624</v>
+      </c>
+      <c r="C85" s="1">
+        <v>45363</v>
       </c>
     </row>
   </sheetData>
@@ -7964,7 +7997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>

</xml_diff>